<commit_message>
adds newline to print
</commit_message>
<xml_diff>
--- a/matches.xlsx
+++ b/matches.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexpiazza/Desktop/get_matches_testing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexpiazza/Desktop/fetching-soccer-matches/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE42B502-2E21-384B-9936-8986662EC8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62F843B-4B0C-CA43-B234-72DF6B6E9F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -454,10 +454,16 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>